<commit_message>
Made concat_variables a function
</commit_message>
<xml_diff>
--- a/grouped_frequencies.xlsx
+++ b/grouped_frequencies.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="17920" windowHeight="10960" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6380" yWindow="500" windowWidth="19420" windowHeight="13060" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -29,11 +29,6 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
@@ -49,27 +44,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -97,15 +77,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -473,54 +450,220 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A1" sqref="A1:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n"/>
-      <c r="B1" s="1" t="n"/>
-      <c r="C1" s="1" t="n"/>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Variable</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value counts</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Total counts</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n"/>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>All other</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.224</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n"/>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Convenience or comfort of use issues</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.008</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n"/>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Hard to start, wouldn't start, shut off</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.056</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n"/>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Issue with gears</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.008</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n"/>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Issue with lights, gauges, panels, latches</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.032</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n"/>
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Issues with clutch, transmission</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.048</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n"/>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Issues with fuel system, fuel tanks</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.008</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n"/>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Issues with hydraulics</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.176</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n"/>
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Issues with seat</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.024</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n"/>
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Issues with tires</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n"/>
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Issues with wiring, electrical</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.016</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n"/>
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Leaking</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.07199999999999999</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Nuts, bolts, parts loose, falling off</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.056</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Oil leak</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Poor quality, flimsy</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.032</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>Slow, hard to get parts and supplies</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.07199999999999999</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>Unacceptable issues for new tractor, not correctly prepared for sale or use</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.048</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>Under powered, needs to be stronger</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.064</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>Total counts</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>125</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -535,31 +678,31 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Variable</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Value counts</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Total counts</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Aftertaste</t>
         </is>
@@ -569,7 +712,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>All other</t>
         </is>
@@ -579,7 +722,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>Citrus, lemon, lime flavor</t>
         </is>
@@ -589,7 +732,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>Flavor, taste</t>
         </is>
@@ -599,7 +742,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>Fruity flavor</t>
         </is>
@@ -609,7 +752,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>Level of flavor, strong, not too strong, not too weak</t>
         </is>
@@ -619,7 +762,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="inlineStr">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>Nothing</t>
         </is>
@@ -629,7 +772,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="inlineStr">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>Refreshing</t>
         </is>
@@ -639,7 +782,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="inlineStr">
+      <c r="A10" s="1" t="inlineStr">
         <is>
           <t>Smooth</t>
         </is>
@@ -649,7 +792,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="inlineStr">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>Sweetness</t>
         </is>
@@ -659,7 +802,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="inlineStr">
+      <c r="A12" s="1" t="inlineStr">
         <is>
           <t>Tangy</t>
         </is>
@@ -669,7 +812,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="inlineStr">
+      <c r="A13" s="1" t="inlineStr">
         <is>
           <t>Total counts</t>
         </is>
@@ -691,31 +834,31 @@
   </sheetPr>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Variable</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Value counts</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Total counts</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>All other</t>
         </is>
@@ -726,7 +869,7 @@
       <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Convenience or comfort of use issues</t>
         </is>
@@ -737,7 +880,7 @@
       <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Hard to start, wouldn't start, shut off</t>
         </is>
@@ -748,7 +891,7 @@
       <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Issue with gears</t>
         </is>
@@ -759,7 +902,7 @@
       <c r="C5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>Issue with lights, gauges, panels, latches</t>
         </is>
@@ -770,7 +913,7 @@
       <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>Issues with clutch, transmission</t>
         </is>
@@ -781,7 +924,7 @@
       <c r="C7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>Issues with fuel system, fuel tanks</t>
         </is>
@@ -792,7 +935,7 @@
       <c r="C8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>Issues with hydraulics</t>
         </is>
@@ -803,7 +946,7 @@
       <c r="C9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>Issues with seat</t>
         </is>
@@ -814,7 +957,7 @@
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>Issues with tires</t>
         </is>
@@ -825,7 +968,7 @@
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>Issues with wiring, electrical</t>
         </is>
@@ -836,7 +979,7 @@
       <c r="C12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>Leaking</t>
         </is>
@@ -847,7 +990,7 @@
       <c r="C13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr">
         <is>
           <t>Nuts, bolts, parts loose, falling off</t>
         </is>
@@ -858,7 +1001,7 @@
       <c r="C14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="inlineStr">
+      <c r="A15" s="2" t="inlineStr">
         <is>
           <t>Oil leak</t>
         </is>
@@ -869,7 +1012,7 @@
       <c r="C15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="inlineStr">
+      <c r="A16" s="2" t="inlineStr">
         <is>
           <t>Poor quality, flimsy</t>
         </is>
@@ -880,7 +1023,7 @@
       <c r="C16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="inlineStr">
+      <c r="A17" s="2" t="inlineStr">
         <is>
           <t>Slow, hard to get parts and supplies</t>
         </is>
@@ -891,7 +1034,7 @@
       <c r="C17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="inlineStr">
+      <c r="A18" s="2" t="inlineStr">
         <is>
           <t>Unacceptable issues for new tractor, not correctly prepared for sale or use</t>
         </is>
@@ -902,7 +1045,7 @@
       <c r="C18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="inlineStr">
+      <c r="A19" s="2" t="inlineStr">
         <is>
           <t>Under powered, needs to be stronger</t>
         </is>
@@ -913,7 +1056,7 @@
       <c r="C19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="inlineStr">
+      <c r="A20" s="2" t="inlineStr">
         <is>
           <t>Total counts</t>
         </is>

</xml_diff>